<commit_message>
Se actualiza el contexto
</commit_message>
<xml_diff>
--- a/generated_skus_catalog.xlsx
+++ b/generated_skus_catalog.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¡Máxima comodidad para tu pequeña! Boxers de algodón Pima, talla 10, suaves y sueltos para todo el día.  Precio por docena: $40.  (Industria Textil Mundo Mágico S.A.C.)</t>
+          <t>¡Comodidad y suavidad para tu pequeña!  Boxers de algodón Pima, talla 10,  sueltos y perfectos para el uso diario.  Precio por docena: $40.  (Industria Textil Mundo Mágico S.A.C.)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>imagen_¡Máxima_comodidad_para_tu_pequ.png</t>
+          <t>imagen_¡Comodidad_y_suavidad_para_tu_.png</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Medias Melcans de algodón, tallas 12-20. ¡Suavidad y comodidad para todo el día!  Precio por docena: $40.  Proveedor: INVERSIONES LENCIMODA S.A.C.</t>
+          <t>Medias Melcans de algodón, tallas 12-20. ¡Suavidad y confort para todo el día!  Precio por docena: $40.  Proveedor: INVERSIONES LENCIMODA S.A.C.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">

</xml_diff>